<commit_message>
Saving output of the fixed T1L and FL
</commit_message>
<xml_diff>
--- a/Lacex_summary_0419_recover_old_try3.xlsx
+++ b/Lacex_summary_0419_recover_old_try3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0C4614-DBB1-475A-8A64-96BCB69E4A64}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5562A5-3FBD-4537-8991-A1F810AA7657}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="2" xr2:uid="{C8260871-5761-403D-B0F9-C73A16D339A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C8260871-5761-403D-B0F9-C73A16D339A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -606,11 +606,97 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-0D45-4EC1-8A36-B03DCDACA9EF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0D45-4EC1-8A36-B03DCDACA9EF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0D45-4EC1-8A36-B03DCDACA9EF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0D45-4EC1-8A36-B03DCDACA9EF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -960,11 +1046,97 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-1E23-456E-8B20-A703430178B2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1E23-456E-8B20-A703430178B2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1E23-456E-8B20-A703430178B2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1E23-456E-8B20-A703430178B2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -1328,11 +1500,97 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-B604-4C8C-8071-C0D5BE90777C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B604-4C8C-8071-C0D5BE90777C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-B604-4C8C-8071-C0D5BE90777C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B604-4C8C-8071-C0D5BE90777C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -6715,16 +6973,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>328986</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>97072</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>168966</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>24186</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>97073</xdr:rowOff>
+      <xdr:colOff>473766</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127553</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6752,15 +7010,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>43815</xdr:rowOff>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>43815</xdr:rowOff>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6788,15 +7046,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>604631</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>663</xdr:rowOff>
+      <xdr:colOff>284591</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>99723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>299831</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>662</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>589391</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>99722</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7540,7 +7798,7 @@
   <dimension ref="A1:AB88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>